<commit_message>
0.1 version - It is working at a very basic level
</commit_message>
<xml_diff>
--- a/data/4-17-22 service plan.xlsx
+++ b/data/4-17-22 service plan.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtt/Projects/VMIX-Helper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D53E09A-A052-0D4E-927A-42D9B4F59791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9708BEE1-BC7A-AE44-AFE0-D9950F3E4F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="3" r:id="rId1"/>
-    <sheet name="Reference" sheetId="4" r:id="rId2"/>
+    <sheet name="vMixConfig" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="FIlteredMediaNumber">Reference!#REF!</definedName>
-    <definedName name="FilteredMediaType">Reference!#REF!</definedName>
-    <definedName name="FilteredShortName">Reference!$T$1</definedName>
-    <definedName name="mediaNumber">OFFSET(Reference!$B:$B,0,0,COUNTA(Reference!$B:$B),1)</definedName>
-    <definedName name="mediaType">OFFSET(Reference!$C:$C,0,0,COUNTA(Reference!$C:$C),1)</definedName>
-    <definedName name="shortTitle">OFFSET(Reference!$E:$E,0,0,COUNTA(Reference!$E:$E),1)</definedName>
-    <definedName name="VMix">Reference!$A:$E</definedName>
-    <definedName name="VMixMediaType">Reference!$C:$C</definedName>
+    <definedName name="FIlteredMediaNumber">vMixConfig!#REF!</definedName>
+    <definedName name="FilteredMediaType">vMixConfig!#REF!</definedName>
+    <definedName name="FilteredShortName">vMixConfig!$T$1</definedName>
+    <definedName name="mediaNumber">OFFSET(vMixConfig!$B:$B,0,0,COUNTA(vMixConfig!$B:$B),1)</definedName>
+    <definedName name="mediaType">OFFSET(vMixConfig!$C:$C,0,0,COUNTA(vMixConfig!$C:$C),1)</definedName>
+    <definedName name="shortTitle">OFFSET(vMixConfig!$E:$E,0,0,COUNTA(vMixConfig!$E:$E),1)</definedName>
+    <definedName name="VMix">vMixConfig!$A:$E</definedName>
+    <definedName name="VMixMediaType">vMixConfig!$C:$C</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="autoNoTable"/>
   <extLst>
@@ -1332,7 +1332,7 @@
   </sheetPr>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
@@ -1399,7 +1399,7 @@
     <row r="2" spans="1:14" ht="15">
       <c r="A2" s="10"/>
       <c r="B2" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F2,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F2,vMixConfig!$E:$E,0))</f>
         <v>13</v>
       </c>
       <c r="C2" s="37" t="s">
@@ -1413,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F2,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F2,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H2" s="27" t="str">
@@ -1430,7 +1430,7 @@
     <row r="3" spans="1:14" ht="15">
       <c r="A3" s="10"/>
       <c r="B3" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F3,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F3,vMixConfig!$E:$E,0))</f>
         <v>37</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -1444,7 +1444,7 @@
         <v>199</v>
       </c>
       <c r="G3" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F3,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F3,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H3" s="27" t="str">
@@ -1467,7 +1467,7 @@
     <row r="4" spans="1:14" ht="28">
       <c r="A4" s="10"/>
       <c r="B4" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F4,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F4,vMixConfig!$E:$E,0))</f>
         <v>38</v>
       </c>
       <c r="C4" s="34" t="s">
@@ -1481,7 +1481,7 @@
         <v>203</v>
       </c>
       <c r="G4" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F4,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F4,vMixConfig!$E:$E,0))</f>
         <v>Photos</v>
       </c>
       <c r="H4" s="27" t="str">
@@ -1500,7 +1500,7 @@
     <row r="5" spans="1:14" ht="16">
       <c r="A5" s="10"/>
       <c r="B5" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F5,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F5,vMixConfig!$E:$E,0))</f>
         <v>34</v>
       </c>
       <c r="C5" s="34" t="s">
@@ -1514,7 +1514,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F5,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F5,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H5" s="27" t="str">
@@ -1531,7 +1531,7 @@
     <row r="6" spans="1:14" ht="15">
       <c r="A6" s="10"/>
       <c r="B6" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F6,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F6,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C6" s="34" t="s">
@@ -1545,7 +1545,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F6,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F6,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H6" s="27" t="str">
@@ -1566,7 +1566,7 @@
     <row r="7" spans="1:14" ht="28" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F7,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F7,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C7" s="34" t="s">
@@ -1580,7 +1580,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F7,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F7,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H7" s="27" t="str">
@@ -1601,7 +1601,7 @@
     <row r="8" spans="1:14" ht="42">
       <c r="A8" s="12"/>
       <c r="B8" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F8,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F8,vMixConfig!$E:$E,0))</f>
         <v>39</v>
       </c>
       <c r="C8" s="34" t="s">
@@ -1615,7 +1615,7 @@
         <v>205</v>
       </c>
       <c r="G8" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F8,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F8,vMixConfig!$E:$E,0))</f>
         <v>Video</v>
       </c>
       <c r="H8" s="27" t="str">
@@ -1640,7 +1640,7 @@
     <row r="9" spans="1:14" ht="16">
       <c r="A9" s="12"/>
       <c r="B9" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F9,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F9,vMixConfig!$E:$E,0))</f>
         <v>21</v>
       </c>
       <c r="C9" s="34" t="s">
@@ -1654,7 +1654,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F9,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F9,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H9" s="27" t="str">
@@ -1675,7 +1675,7 @@
     <row r="10" spans="1:14" ht="28">
       <c r="A10" s="12"/>
       <c r="B10" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F10,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F10,vMixConfig!$E:$E,0))</f>
         <v>35</v>
       </c>
       <c r="C10" s="34" t="s">
@@ -1689,7 +1689,7 @@
         <v>20</v>
       </c>
       <c r="G10" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F10,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F10,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H10" s="27" t="str">
@@ -1714,7 +1714,7 @@
     <row r="11" spans="1:14" ht="15">
       <c r="A11" s="12"/>
       <c r="B11" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F11,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F11,vMixConfig!$E:$E,0))</f>
         <v>44</v>
       </c>
       <c r="C11" s="34" t="s">
@@ -1728,7 +1728,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F11,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F11,vMixConfig!$E:$E,0))</f>
         <v>VirtualSet</v>
       </c>
       <c r="H11" s="27" t="str">
@@ -1745,7 +1745,7 @@
     <row r="12" spans="1:14" ht="15">
       <c r="A12" s="12"/>
       <c r="B12" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F12,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F12,vMixConfig!$E:$E,0))</f>
         <v>33</v>
       </c>
       <c r="C12" s="34" t="s">
@@ -1759,7 +1759,7 @@
         <v>26</v>
       </c>
       <c r="G12" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F12,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F12,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H12" s="27" t="str">
@@ -1780,7 +1780,7 @@
     <row r="13" spans="1:14" ht="42">
       <c r="A13" s="12"/>
       <c r="B13" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F13,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F13,vMixConfig!$E:$E,0))</f>
         <v>41</v>
       </c>
       <c r="C13" s="34" t="s">
@@ -1794,7 +1794,7 @@
         <v>212</v>
       </c>
       <c r="G13" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F13,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F13,vMixConfig!$E:$E,0))</f>
         <v>PowerPoint</v>
       </c>
       <c r="H13" s="27" t="str">
@@ -1819,7 +1819,7 @@
     <row r="14" spans="1:14" ht="16">
       <c r="A14" s="12"/>
       <c r="B14" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F14,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F14,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C14" s="34" t="s">
@@ -1833,7 +1833,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F14,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F14,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H14" s="27" t="str">
@@ -1850,7 +1850,7 @@
     <row r="15" spans="1:14" ht="42">
       <c r="A15" s="12"/>
       <c r="B15" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F15,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F15,vMixConfig!$E:$E,0))</f>
         <v>42</v>
       </c>
       <c r="C15" s="34" t="s">
@@ -1864,7 +1864,7 @@
         <v>215</v>
       </c>
       <c r="G15" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F15,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F15,vMixConfig!$E:$E,0))</f>
         <v>PowerPoint</v>
       </c>
       <c r="H15" s="27" t="str">
@@ -1889,7 +1889,7 @@
     <row r="16" spans="1:14" ht="15">
       <c r="A16" s="12"/>
       <c r="B16" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F16,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F16,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C16" s="34" t="s">
@@ -1903,7 +1903,7 @@
         <v>35</v>
       </c>
       <c r="G16" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F16,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F16,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H16" s="27" t="str">
@@ -1920,7 +1920,7 @@
     <row r="17" spans="1:14" ht="28">
       <c r="A17" s="12"/>
       <c r="B17" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F17,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F17,vMixConfig!$E:$E,0))</f>
         <v>45</v>
       </c>
       <c r="C17" s="34" t="s">
@@ -1934,7 +1934,7 @@
         <v>221</v>
       </c>
       <c r="G17" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F17,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F17,vMixConfig!$E:$E,0))</f>
         <v>PowerPoint</v>
       </c>
       <c r="H17" s="27" t="str">
@@ -1959,7 +1959,7 @@
     <row r="18" spans="1:14" s="31" customFormat="1" ht="28">
       <c r="A18" s="12"/>
       <c r="B18" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F18,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F18,vMixConfig!$E:$E,0))</f>
         <v>14</v>
       </c>
       <c r="C18" s="34" t="s">
@@ -1975,7 +1975,7 @@
         <v>137</v>
       </c>
       <c r="G18" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F18,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F18,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H18" s="27" t="str">
@@ -1992,7 +1992,7 @@
     <row r="19" spans="1:14" ht="28">
       <c r="A19" s="12"/>
       <c r="B19" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F19,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F19,vMixConfig!$E:$E,0))</f>
         <v>30</v>
       </c>
       <c r="C19" s="34" t="s">
@@ -2006,7 +2006,7 @@
         <v>181</v>
       </c>
       <c r="G19" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F19,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F19,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H19" s="27" t="str">
@@ -2023,7 +2023,7 @@
     <row r="20" spans="1:14" ht="42">
       <c r="A20" s="12"/>
       <c r="B20" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F20,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F20,vMixConfig!$E:$E,0))</f>
         <v>43</v>
       </c>
       <c r="C20" s="37" t="s">
@@ -2037,7 +2037,7 @@
         <v>39</v>
       </c>
       <c r="G20" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F20,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F20,vMixConfig!$E:$E,0))</f>
         <v>Colour</v>
       </c>
       <c r="H20" s="27" t="str">
@@ -2060,7 +2060,7 @@
     <row r="21" spans="1:14" ht="28">
       <c r="A21" s="12"/>
       <c r="B21" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F21,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F21,vMixConfig!$E:$E,0))</f>
         <v>14</v>
       </c>
       <c r="C21" s="34" t="s">
@@ -2074,7 +2074,7 @@
         <v>137</v>
       </c>
       <c r="G21" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F21,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F21,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H21" s="27" t="str">
@@ -2099,7 +2099,7 @@
     <row r="22" spans="1:14" ht="28">
       <c r="A22" s="12"/>
       <c r="B22" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F22,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F22,vMixConfig!$E:$E,0))</f>
         <v>33</v>
       </c>
       <c r="C22" s="38" t="s">
@@ -2113,7 +2113,7 @@
         <v>47</v>
       </c>
       <c r="G22" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F22,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F22,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H22" s="27" t="str">
@@ -2134,7 +2134,7 @@
     <row r="23" spans="1:14" ht="42">
       <c r="A23" s="12"/>
       <c r="B23" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F23,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F23,vMixConfig!$E:$E,0))</f>
         <v>26</v>
       </c>
       <c r="C23" s="34" t="s">
@@ -2148,7 +2148,7 @@
         <v>49</v>
       </c>
       <c r="G23" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F23,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F23,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H23" s="27" t="str">
@@ -2171,7 +2171,7 @@
     <row r="24" spans="1:14" ht="16">
       <c r="A24" s="12"/>
       <c r="B24" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F24,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F24,vMixConfig!$E:$E,0))</f>
         <v>34</v>
       </c>
       <c r="C24" s="34" t="s">
@@ -2187,7 +2187,7 @@
         <v>8</v>
       </c>
       <c r="G24" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F24,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F24,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H24" s="27" t="str">
@@ -2204,7 +2204,7 @@
     <row r="25" spans="1:14" ht="16">
       <c r="A25" s="12"/>
       <c r="B25" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F25,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F25,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C25" s="34" t="s">
@@ -2218,7 +2218,7 @@
         <v>35</v>
       </c>
       <c r="G25" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F25,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F25,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H25" s="27" t="str">
@@ -2239,7 +2239,7 @@
     <row r="26" spans="1:14" ht="28" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F26,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F26,vMixConfig!$E:$E,0))</f>
         <v>46</v>
       </c>
       <c r="C26" s="37" t="s">
@@ -2251,7 +2251,7 @@
         <v>224</v>
       </c>
       <c r="G26" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F26,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F26,vMixConfig!$E:$E,0))</f>
         <v>GT</v>
       </c>
       <c r="H26" s="27" t="str">
@@ -2270,7 +2270,7 @@
     <row r="27" spans="1:14" ht="28">
       <c r="A27" s="12"/>
       <c r="B27" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F27,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F27,vMixConfig!$E:$E,0))</f>
         <v>37</v>
       </c>
       <c r="C27" s="38" t="s">
@@ -2284,7 +2284,7 @@
         <v>199</v>
       </c>
       <c r="G27" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F27,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F27,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H27" s="27" t="str">
@@ -2307,7 +2307,7 @@
     <row r="28" spans="1:14" ht="15">
       <c r="A28" s="12"/>
       <c r="B28" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F28,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F28,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C28" s="38" t="s">
@@ -2321,7 +2321,7 @@
         <v>9</v>
       </c>
       <c r="G28" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F28,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F28,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H28" s="27" t="str">
@@ -2338,7 +2338,7 @@
     <row r="29" spans="1:14" ht="28">
       <c r="A29" s="12"/>
       <c r="B29" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F29,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F29,vMixConfig!$E:$E,0))</f>
         <v>48</v>
       </c>
       <c r="C29" s="38" t="s">
@@ -2352,7 +2352,7 @@
         <v>231</v>
       </c>
       <c r="G29" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F29,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F29,vMixConfig!$E:$E,0))</f>
         <v>PowerPoint</v>
       </c>
       <c r="H29" s="27" t="str">
@@ -2375,7 +2375,7 @@
     <row r="30" spans="1:14" ht="15">
       <c r="A30" s="12"/>
       <c r="B30" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F30,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F30,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C30" s="34" t="s">
@@ -2389,7 +2389,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F30,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F30,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H30" s="27" t="str">
@@ -2406,7 +2406,7 @@
     <row r="31" spans="1:14" ht="15">
       <c r="A31" s="12"/>
       <c r="B31" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F31,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F31,vMixConfig!$E:$E,0))</f>
         <v>37</v>
       </c>
       <c r="C31" s="34" t="s">
@@ -2420,7 +2420,7 @@
         <v>199</v>
       </c>
       <c r="G31" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F31,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F31,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H31" s="27" t="str">
@@ -2443,7 +2443,7 @@
     <row r="32" spans="1:14" ht="15">
       <c r="A32" s="12"/>
       <c r="B32" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F32,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F32,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C32" s="34" t="s">
@@ -2457,7 +2457,7 @@
         <v>9</v>
       </c>
       <c r="G32" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F32,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F32,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H32" s="27" t="str">
@@ -2474,7 +2474,7 @@
     <row r="33" spans="1:14" ht="28">
       <c r="A33" s="12"/>
       <c r="B33" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F33,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F33,vMixConfig!$E:$E,0))</f>
         <v>49</v>
       </c>
       <c r="C33" s="34" t="s">
@@ -2488,7 +2488,7 @@
         <v>234</v>
       </c>
       <c r="G33" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F33,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F33,vMixConfig!$E:$E,0))</f>
         <v>PowerPoint</v>
       </c>
       <c r="H33" s="27" t="str">
@@ -2511,7 +2511,7 @@
     <row r="34" spans="1:14" ht="15">
       <c r="A34" s="12"/>
       <c r="B34" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F34,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F34,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C34" s="34" t="s">
@@ -2525,7 +2525,7 @@
         <v>9</v>
       </c>
       <c r="G34" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F34,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F34,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H34" s="27" t="str">
@@ -2542,7 +2542,7 @@
     <row r="35" spans="1:14" ht="29">
       <c r="A35" s="12"/>
       <c r="B35" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F35,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F35,vMixConfig!$E:$E,0))</f>
         <v>36</v>
       </c>
       <c r="C35" s="34" t="s">
@@ -2556,7 +2556,7 @@
         <v>196</v>
       </c>
       <c r="G35" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F35,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F35,vMixConfig!$E:$E,0))</f>
         <v>VirtualSet</v>
       </c>
       <c r="H35" s="27" t="str">
@@ -2583,7 +2583,7 @@
     <row r="36" spans="1:14" ht="15">
       <c r="A36" s="12"/>
       <c r="B36" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F36,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F36,vMixConfig!$E:$E,0))</f>
         <v>44</v>
       </c>
       <c r="C36" s="34" t="s">
@@ -2597,7 +2597,7 @@
         <v>65</v>
       </c>
       <c r="G36" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F36,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F36,vMixConfig!$E:$E,0))</f>
         <v>VirtualSet</v>
       </c>
       <c r="H36" s="27" t="str">
@@ -2616,7 +2616,7 @@
     <row r="37" spans="1:14" ht="29">
       <c r="A37" s="12"/>
       <c r="B37" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F37,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F37,vMixConfig!$E:$E,0))</f>
         <v>44</v>
       </c>
       <c r="C37" s="34" t="s">
@@ -2630,7 +2630,7 @@
         <v>25</v>
       </c>
       <c r="G37" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F37,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F37,vMixConfig!$E:$E,0))</f>
         <v>VirtualSet</v>
       </c>
       <c r="H37" s="27" t="str">
@@ -2657,7 +2657,7 @@
     <row r="38" spans="1:14" ht="29">
       <c r="A38" s="12"/>
       <c r="B38" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F38,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F38,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C38" s="34" t="s">
@@ -2671,7 +2671,7 @@
         <v>9</v>
       </c>
       <c r="G38" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F38,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F38,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H38" s="27" t="str">
@@ -2696,7 +2696,7 @@
     <row r="39" spans="1:14" ht="15">
       <c r="A39" s="12"/>
       <c r="B39" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F39,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F39,vMixConfig!$E:$E,0))</f>
         <v>34</v>
       </c>
       <c r="C39" s="34" t="s">
@@ -2710,7 +2710,7 @@
         <v>72</v>
       </c>
       <c r="G39" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F39,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F39,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H39" s="27" t="str">
@@ -2729,7 +2729,7 @@
     <row r="40" spans="1:14" ht="15">
       <c r="A40" s="12"/>
       <c r="B40" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F40,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F40,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C40" s="34" t="s">
@@ -2743,7 +2743,7 @@
         <v>9</v>
       </c>
       <c r="G40" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F40,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F40,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H40" s="27" t="str">
@@ -2762,7 +2762,7 @@
     <row r="41" spans="1:14" ht="42">
       <c r="A41" s="10"/>
       <c r="B41" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F41,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F41,vMixConfig!$E:$E,0))</f>
         <v>50</v>
       </c>
       <c r="C41" s="34" t="s">
@@ -2776,7 +2776,7 @@
         <v>237</v>
       </c>
       <c r="G41" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F41,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F41,vMixConfig!$E:$E,0))</f>
         <v>PowerPoint</v>
       </c>
       <c r="H41" s="27" t="str">
@@ -2801,7 +2801,7 @@
     <row r="42" spans="1:14" ht="28">
       <c r="A42" s="10"/>
       <c r="B42" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F42,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F42,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C42" s="34" t="s">
@@ -2815,7 +2815,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F42,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F42,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H42" s="27" t="str">
@@ -2836,7 +2836,7 @@
     <row r="43" spans="1:14" ht="28">
       <c r="A43" s="10"/>
       <c r="B43" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F43,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F43,vMixConfig!$E:$E,0))</f>
         <v>51</v>
       </c>
       <c r="C43" s="38" t="s">
@@ -2850,7 +2850,7 @@
         <v>240</v>
       </c>
       <c r="G43" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F43,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F43,vMixConfig!$E:$E,0))</f>
         <v>Image</v>
       </c>
       <c r="H43" s="27" t="str">
@@ -2869,7 +2869,7 @@
     <row r="44" spans="1:14" ht="16">
       <c r="A44" s="10"/>
       <c r="B44" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F44,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F44,vMixConfig!$E:$E,0))</f>
         <v>19</v>
       </c>
       <c r="C44" s="34" t="s">
@@ -2883,7 +2883,7 @@
         <v>9</v>
       </c>
       <c r="G44" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F44,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F44,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H44" s="27" t="str">
@@ -2904,7 +2904,7 @@
     <row r="45" spans="1:14" ht="16">
       <c r="A45" s="10"/>
       <c r="B45" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F45,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F45,vMixConfig!$E:$E,0))</f>
         <v>37</v>
       </c>
       <c r="C45" s="34" t="s">
@@ -2918,7 +2918,7 @@
         <v>199</v>
       </c>
       <c r="G45" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F45,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F45,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H45" s="27" t="str">
@@ -2939,7 +2939,7 @@
     <row r="46" spans="1:14" ht="16">
       <c r="A46" s="10"/>
       <c r="B46" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F46,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F46,vMixConfig!$E:$E,0))</f>
         <v>13</v>
       </c>
       <c r="C46" s="34" t="s">
@@ -2953,7 +2953,7 @@
         <v>133</v>
       </c>
       <c r="G46" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F46,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F46,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H46" s="27" t="str">
@@ -2972,7 +2972,7 @@
     <row r="47" spans="1:14" ht="16">
       <c r="A47" s="10"/>
       <c r="B47" s="27">
-        <f>INDEX(Reference!B:B,MATCH(F47,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!B:B,MATCH(F47,vMixConfig!$E:$E,0))</f>
         <v>37</v>
       </c>
       <c r="C47" s="34" t="s">
@@ -2986,7 +2986,7 @@
         <v>199</v>
       </c>
       <c r="G47" s="27" t="str">
-        <f>INDEX(Reference!C:C,MATCH(F47,Reference!$E:$E,0))</f>
+        <f>INDEX(vMixConfig!C:C,MATCH(F47,vMixConfig!$E:$E,0))</f>
         <v>Virtual</v>
       </c>
       <c r="H47" s="27" t="str">
@@ -3183,7 +3183,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{064A5871-2883-674A-836C-90AA981EF0DC}">
           <x14:formula1>
-            <xm:f>Reference!$T:$T</xm:f>
+            <xm:f>vMixConfig!$T:$T</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F47</xm:sqref>
         </x14:dataValidation>
@@ -3197,7 +3197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2EE200-2F6B-A74A-A266-8BF3F2F1ADCB}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>

</xml_diff>